<commit_message>
Finished Inventory Reporting and Management
</commit_message>
<xml_diff>
--- a/utilities/UpdateInventory.xlsx
+++ b/utilities/UpdateInventory.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="183">
   <si>
     <t>TOTAL</t>
   </si>
@@ -1560,7 +1560,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1664,77 +1664,65 @@
       <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="25">
+      <c r="B9" s="23"/>
+      <c r="C9" s="25" t="str">
         <f>_xlfn.IFNA(INDEX(Product!$A$1:$J$78,MATCH(SimpleInvoice[[#This Row],[Product Name]],Product!$B$1:$B$78,FALSE),1)," ")</f>
-        <v>10</v>
-      </c>
-      <c r="D9" s="24">
-        <v>-30</v>
-      </c>
-      <c r="E9" s="13">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D9" s="24"/>
+      <c r="E9" s="13" t="str">
         <f>_xlfn.IFNA(INDEX(Product!$A$1:$J$78,MATCH(SimpleInvoice[[#This Row],[Product Name]],Product!$B$1:$B$78,FALSE),6)," ")</f>
-        <v>31</v>
-      </c>
-      <c r="F9" s="12" t="b">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F9" s="12" t="str">
         <f>_xlfn.IFNA(INDEX(Product!$A$1:$J$78,MATCH(SimpleInvoice[[#This Row],[Product Name]],Product!$B$1:$B$78,FALSE),10)," ")</f>
-        <v>0</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G9" s="13">
         <f>IFERROR(SimpleInvoice[[#This Row],[Quantity ( + / - )]]*SimpleInvoice[[#This Row],[Price]],0)</f>
-        <v>-930</v>
+        <v>0</v>
       </c>
       <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="25">
+      <c r="B10" s="23"/>
+      <c r="C10" s="25" t="str">
         <f>_xlfn.IFNA(INDEX(Product!$A$1:$J$78,MATCH(SimpleInvoice[[#This Row],[Product Name]],Product!$B$1:$B$78,FALSE),1)," ")</f>
-        <v>1</v>
-      </c>
-      <c r="D10" s="24">
-        <v>16</v>
-      </c>
-      <c r="E10" s="13">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="13" t="str">
         <f>_xlfn.IFNA(INDEX(Product!$A$1:$J$78,MATCH(SimpleInvoice[[#This Row],[Product Name]],Product!$B$1:$B$78,FALSE),6)," ")</f>
-        <v>18</v>
-      </c>
-      <c r="F10" s="12" t="b">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F10" s="12" t="str">
         <f>_xlfn.IFNA(INDEX(Product!$A$1:$J$78,MATCH(SimpleInvoice[[#This Row],[Product Name]],Product!$B$1:$B$78,FALSE),10)," ")</f>
-        <v>0</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G10" s="13">
         <f>IFERROR(SimpleInvoice[[#This Row],[Quantity ( + / - )]]*SimpleInvoice[[#This Row],[Price]],0)</f>
-        <v>288</v>
+        <v>0</v>
       </c>
       <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="25">
+      <c r="B11" s="23"/>
+      <c r="C11" s="25" t="str">
         <f>_xlfn.IFNA(INDEX(Product!$A$1:$J$78,MATCH(SimpleInvoice[[#This Row],[Product Name]],Product!$B$1:$B$78,FALSE),1)," ")</f>
-        <v>26</v>
-      </c>
-      <c r="D11" s="24">
-        <v>45</v>
-      </c>
-      <c r="E11" s="13">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="13" t="str">
         <f>_xlfn.IFNA(INDEX(Product!$A$1:$J$78,MATCH(SimpleInvoice[[#This Row],[Product Name]],Product!$B$1:$B$78,FALSE),6)," ")</f>
-        <v>31.23</v>
-      </c>
-      <c r="F11" s="12" t="b">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F11" s="12" t="str">
         <f>_xlfn.IFNA(INDEX(Product!$A$1:$J$78,MATCH(SimpleInvoice[[#This Row],[Product Name]],Product!$B$1:$B$78,FALSE),10)," ")</f>
-        <v>0</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G11" s="13">
         <f>IFERROR(SimpleInvoice[[#This Row],[Quantity ( + / - )]]*SimpleInvoice[[#This Row],[Price]],0)</f>
-        <v>1405.35</v>
+        <v>0</v>
       </c>
       <c r="H11" s="22"/>
     </row>
@@ -1946,7 +1934,7 @@
       </c>
       <c r="G22" s="14">
         <f>SUM(SimpleInvoice[Inventory ∆])</f>
-        <v>763.34999999999991</v>
+        <v>0</v>
       </c>
       <c r="H22" s="21"/>
     </row>

</xml_diff>

<commit_message>
Initialize Assets Dashboard using data from Inventory Reporting
</commit_message>
<xml_diff>
--- a/utilities/UpdateInventory.xlsx
+++ b/utilities/UpdateInventory.xlsx
@@ -1000,6 +1000,21 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="3" xfId="16" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="0" xfId="16" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="7" applyBorder="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="7" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="7" applyBorder="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="15" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -1023,21 +1038,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="3" xfId="16" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="0" xfId="16" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="7" applyBorder="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="7" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="7" applyBorder="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1560,7 +1560,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1589,46 +1589,46 @@
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="15"/>
       <c r="C4" s="28"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
       <c r="F4" s="8"/>
       <c r="G4" s="29"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="41"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
       <c r="F5" s="8"/>
       <c r="G5" s="30"/>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="41"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
       <c r="F6" s="28"/>
       <c r="G6" s="3"/>
       <c r="H6" s="2"/>
@@ -1672,7 +1672,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="24">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="E9" s="13">
         <f>_xlfn.IFNA(INDEX(Product!$A$1:$J$78,MATCH(SimpleInvoice[[#This Row],[Product Name]],Product!$B$1:$B$78,FALSE),6)," ")</f>
@@ -1684,7 +1684,7 @@
       </c>
       <c r="G9" s="13">
         <f>IFERROR(SimpleInvoice[[#This Row],[Quantity ( + / - )]]*SimpleInvoice[[#This Row],[Price]],0)</f>
-        <v>1782</v>
+        <v>1350</v>
       </c>
       <c r="H9" s="22"/>
     </row>
@@ -1920,37 +1920,31 @@
       <c r="H20" s="22"/>
     </row>
     <row r="21" spans="2:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="37"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="42"/>
       <c r="F21" s="26"/>
       <c r="G21" s="27"/>
       <c r="H21" s="22"/>
     </row>
     <row r="22" spans="2:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="35"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="40"/>
       <c r="F22" s="7" t="s">
         <v>0</v>
       </c>
       <c r="G22" s="14">
         <f>SUM(SimpleInvoice[Inventory ∆])</f>
-        <v>1782</v>
+        <v>1350</v>
       </c>
       <c r="H22" s="21"/>
     </row>
   </sheetData>
   <sheetProtection password="ED6A" sheet="1" objects="1" scenarios="1" selectLockedCells="1" sort="0"/>
   <mergeCells count="13">
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="D4:E4"/>
@@ -1958,6 +1952,12 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F21">

</xml_diff>